<commit_message>
trabalho final finalizado :)
</commit_message>
<xml_diff>
--- a/trabalho_final/custos_talhao_103_parcela_196.xlsx
+++ b/trabalho_final/custos_talhao_103_parcela_196.xlsx
@@ -8,13 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\OppenSocial\Desktop\manejo_plantadas\trabalho_final\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A10785C-5062-40F9-96A0-492B1D215D66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CC79339-8C25-402A-9EA4-14825EA962FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22365" yWindow="1575" windowWidth="14310" windowHeight="12225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="21990" yWindow="435" windowWidth="14310" windowHeight="15015" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="custos_talhao_103_parcela_196" sheetId="1" r:id="rId1"/>
+    <sheet name="Plan2" sheetId="2" r:id="rId2"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId3"/>
+  </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -33,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>Terra (R$/ha)</t>
   </si>
@@ -108,6 +112,21 @@
   </si>
   <si>
     <t>Colheita  (R$/m³) e Despesas adm.</t>
+  </si>
+  <si>
+    <t>projeto</t>
+  </si>
+  <si>
+    <t>idade</t>
+  </si>
+  <si>
+    <t>custo</t>
+  </si>
+  <si>
+    <t>receita</t>
+  </si>
+  <si>
+    <t>producao</t>
   </si>
 </sst>
 </file>
@@ -591,9 +610,10 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Ênfase1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -650,6 +670,200 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Plan1"/>
+      <sheetName val="Plan2"/>
+      <sheetName val="Plan3"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="11">
+          <cell r="B11">
+            <v>6000</v>
+          </cell>
+          <cell r="C11">
+            <v>6000</v>
+          </cell>
+          <cell r="D11">
+            <v>6000</v>
+          </cell>
+          <cell r="E11">
+            <v>6000</v>
+          </cell>
+          <cell r="F11">
+            <v>6000</v>
+          </cell>
+          <cell r="G11">
+            <v>6000</v>
+          </cell>
+          <cell r="H11">
+            <v>6000</v>
+          </cell>
+          <cell r="I11">
+            <v>6000</v>
+          </cell>
+        </row>
+        <row r="12">
+          <cell r="B12">
+            <v>290</v>
+          </cell>
+          <cell r="C12">
+            <v>290</v>
+          </cell>
+          <cell r="D12">
+            <v>290</v>
+          </cell>
+          <cell r="E12">
+            <v>290</v>
+          </cell>
+          <cell r="F12">
+            <v>290</v>
+          </cell>
+          <cell r="G12">
+            <v>290</v>
+          </cell>
+          <cell r="H12">
+            <v>290</v>
+          </cell>
+          <cell r="I12">
+            <v>290</v>
+          </cell>
+        </row>
+        <row r="13">
+          <cell r="B13">
+            <v>140</v>
+          </cell>
+          <cell r="C13">
+            <v>140</v>
+          </cell>
+          <cell r="D13">
+            <v>140</v>
+          </cell>
+          <cell r="E13">
+            <v>140</v>
+          </cell>
+          <cell r="F13">
+            <v>140</v>
+          </cell>
+          <cell r="G13">
+            <v>140</v>
+          </cell>
+          <cell r="H13">
+            <v>140</v>
+          </cell>
+          <cell r="I13">
+            <v>140</v>
+          </cell>
+        </row>
+        <row r="14">
+          <cell r="C14">
+            <v>40</v>
+          </cell>
+          <cell r="D14">
+            <v>40</v>
+          </cell>
+          <cell r="E14">
+            <v>40</v>
+          </cell>
+          <cell r="F14">
+            <v>40</v>
+          </cell>
+          <cell r="G14">
+            <v>40</v>
+          </cell>
+          <cell r="H14">
+            <v>40</v>
+          </cell>
+          <cell r="I14">
+            <v>40</v>
+          </cell>
+        </row>
+        <row r="15">
+          <cell r="D15">
+            <v>40</v>
+          </cell>
+          <cell r="E15">
+            <v>40</v>
+          </cell>
+          <cell r="F15">
+            <v>40</v>
+          </cell>
+          <cell r="G15">
+            <v>40</v>
+          </cell>
+          <cell r="H15">
+            <v>40</v>
+          </cell>
+          <cell r="I15">
+            <v>40</v>
+          </cell>
+        </row>
+        <row r="16">
+          <cell r="E16">
+            <v>40</v>
+          </cell>
+          <cell r="F16">
+            <v>40</v>
+          </cell>
+          <cell r="G16">
+            <v>40</v>
+          </cell>
+          <cell r="H16">
+            <v>40</v>
+          </cell>
+          <cell r="I16">
+            <v>40</v>
+          </cell>
+        </row>
+        <row r="17">
+          <cell r="F17">
+            <v>40</v>
+          </cell>
+          <cell r="G17">
+            <v>40</v>
+          </cell>
+          <cell r="H17">
+            <v>40</v>
+          </cell>
+          <cell r="I17">
+            <v>40</v>
+          </cell>
+        </row>
+        <row r="18">
+          <cell r="G18">
+            <v>40</v>
+          </cell>
+          <cell r="H18">
+            <v>40</v>
+          </cell>
+          <cell r="I18">
+            <v>40</v>
+          </cell>
+        </row>
+        <row r="19">
+          <cell r="H19">
+            <v>40</v>
+          </cell>
+          <cell r="I19">
+            <v>40</v>
+          </cell>
+        </row>
+        <row r="20">
+          <cell r="I20">
+            <v>40</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -949,10 +1163,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I32"/>
+  <dimension ref="A1:I46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A33" sqref="A33:I46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1131,11 +1345,11 @@
         <v>0</v>
       </c>
       <c r="B11">
+        <f>$C$2</f>
+        <v>8000</v>
+      </c>
+      <c r="C11">
         <f t="shared" ref="B11:I11" si="1">$C$2</f>
-        <v>8000</v>
-      </c>
-      <c r="C11">
-        <f t="shared" si="1"/>
         <v>8000</v>
       </c>
       <c r="D11">
@@ -1818,6 +2032,1178 @@
       <c r="I32">
         <f t="shared" si="14"/>
         <v>-6197.0253625423302</v>
+      </c>
+    </row>
+    <row r="35" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="F35" s="2"/>
+      <c r="G35" s="2"/>
+    </row>
+    <row r="36" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="F36" s="2"/>
+      <c r="G36" s="2"/>
+    </row>
+    <row r="37" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="F37" s="2"/>
+      <c r="G37" s="2"/>
+    </row>
+    <row r="38" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="F38" s="2"/>
+      <c r="G38" s="2"/>
+    </row>
+    <row r="39" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="F39" s="2"/>
+      <c r="G39" s="2"/>
+    </row>
+    <row r="40" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="F40" s="2"/>
+      <c r="G40" s="2"/>
+    </row>
+    <row r="41" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="G41" s="2"/>
+    </row>
+    <row r="42" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E42" s="2"/>
+      <c r="F42" s="2"/>
+      <c r="G42" s="2"/>
+    </row>
+    <row r="43" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="G43" s="2"/>
+    </row>
+    <row r="44" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="G44" s="2"/>
+    </row>
+    <row r="45" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="G45" s="2"/>
+    </row>
+    <row r="46" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="G46" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3C85B8A-D4BB-4492-A12E-2E1DF4687898}">
+  <dimension ref="A1:E61"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>3</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <f>[1]Plan1!B11</f>
+        <v>6000</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>3</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <f>[1]Plan1!B12</f>
+        <v>290</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4">
+        <f>[1]Plan1!B13</f>
+        <v>140</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>3</v>
+      </c>
+      <c r="C5">
+        <f>custos_talhao_103_parcela_196!B14</f>
+        <v>12204.77782685025</v>
+      </c>
+      <c r="D5">
+        <f>custos_talhao_103_parcela_196!B22</f>
+        <v>26032.792427643119</v>
+      </c>
+      <c r="E5">
+        <f>custos_talhao_103_parcela_196!B7</f>
+        <v>185.948517340308</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <f>[1]Plan1!C11</f>
+        <v>6000</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>4</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <f>[1]Plan1!C12</f>
+        <v>290</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>4</v>
+      </c>
+      <c r="B8">
+        <v>2</v>
+      </c>
+      <c r="C8">
+        <f>[1]Plan1!C13</f>
+        <v>140</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>4</v>
+      </c>
+      <c r="B9">
+        <v>3</v>
+      </c>
+      <c r="C9">
+        <f>[1]Plan1!C14</f>
+        <v>40</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>4</v>
+      </c>
+      <c r="B10">
+        <v>4</v>
+      </c>
+      <c r="C10">
+        <f>custos_talhao_103_parcela_196!C15</f>
+        <v>17057.283713704943</v>
+      </c>
+      <c r="D10">
+        <f>custos_talhao_103_parcela_196!C22</f>
+        <v>37944.807989776244</v>
+      </c>
+      <c r="E10">
+        <f>custos_talhao_103_parcela_196!C7</f>
+        <v>271.03434278411601</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>5</v>
+      </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <f>[1]Plan1!D11</f>
+        <v>6000</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>5</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12">
+        <f>[1]Plan1!D12</f>
+        <v>290</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>5</v>
+      </c>
+      <c r="B13">
+        <v>2</v>
+      </c>
+      <c r="C13">
+        <f>[1]Plan1!D13</f>
+        <v>140</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>5</v>
+      </c>
+      <c r="B14">
+        <v>3</v>
+      </c>
+      <c r="C14">
+        <f>[1]Plan1!D14</f>
+        <v>40</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>5</v>
+      </c>
+      <c r="B15">
+        <v>4</v>
+      </c>
+      <c r="C15">
+        <f>[1]Plan1!D15</f>
+        <v>40</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>5</v>
+      </c>
+      <c r="B16">
+        <v>5</v>
+      </c>
+      <c r="C16" s="2">
+        <f>custos_talhao_103_parcela_196!D16</f>
+        <v>20978.142299372572</v>
+      </c>
+      <c r="D16">
+        <f>custos_talhao_103_parcela_196!D22</f>
+        <v>47569.799608213958</v>
+      </c>
+      <c r="E16">
+        <f>custos_talhao_103_parcela_196!D7</f>
+        <v>339.784282915814</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>6</v>
+      </c>
+      <c r="B17">
+        <v>0</v>
+      </c>
+      <c r="C17">
+        <f>[1]Plan1!E11</f>
+        <v>6000</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>6</v>
+      </c>
+      <c r="B18">
+        <v>1</v>
+      </c>
+      <c r="C18">
+        <f>[1]Plan1!E12</f>
+        <v>290</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+      <c r="E18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>6</v>
+      </c>
+      <c r="B19">
+        <v>2</v>
+      </c>
+      <c r="C19">
+        <f>[1]Plan1!E13</f>
+        <v>140</v>
+      </c>
+      <c r="D19">
+        <v>0</v>
+      </c>
+      <c r="E19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>6</v>
+      </c>
+      <c r="B20">
+        <v>3</v>
+      </c>
+      <c r="C20">
+        <f>[1]Plan1!E14</f>
+        <v>40</v>
+      </c>
+      <c r="D20">
+        <v>0</v>
+      </c>
+      <c r="E20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>6</v>
+      </c>
+      <c r="B21">
+        <v>4</v>
+      </c>
+      <c r="C21">
+        <f>[1]Plan1!E15</f>
+        <v>40</v>
+      </c>
+      <c r="D21">
+        <v>0</v>
+      </c>
+      <c r="E21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>6</v>
+      </c>
+      <c r="B22">
+        <v>5</v>
+      </c>
+      <c r="C22">
+        <f>[1]Plan1!E16</f>
+        <v>40</v>
+      </c>
+      <c r="D22">
+        <v>0</v>
+      </c>
+      <c r="E22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>6</v>
+      </c>
+      <c r="B23">
+        <v>6</v>
+      </c>
+      <c r="C23">
+        <f>custos_talhao_103_parcela_196!E17</f>
+        <v>24130.18627142076</v>
+      </c>
+      <c r="D23">
+        <f>custos_talhao_103_parcela_196!E22</f>
+        <v>55307.4917868634</v>
+      </c>
+      <c r="E23">
+        <f>custos_talhao_103_parcela_196!E7</f>
+        <v>395.05351276330998</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>7</v>
+      </c>
+      <c r="B24">
+        <v>0</v>
+      </c>
+      <c r="C24">
+        <f>[1]Plan1!F11</f>
+        <v>6000</v>
+      </c>
+      <c r="D24">
+        <v>0</v>
+      </c>
+      <c r="E24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>7</v>
+      </c>
+      <c r="B25">
+        <v>1</v>
+      </c>
+      <c r="C25">
+        <f>[1]Plan1!F12</f>
+        <v>290</v>
+      </c>
+      <c r="D25">
+        <v>0</v>
+      </c>
+      <c r="E25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>7</v>
+      </c>
+      <c r="B26">
+        <v>2</v>
+      </c>
+      <c r="C26">
+        <f>[1]Plan1!F13</f>
+        <v>140</v>
+      </c>
+      <c r="D26">
+        <v>0</v>
+      </c>
+      <c r="E26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>7</v>
+      </c>
+      <c r="B27">
+        <v>3</v>
+      </c>
+      <c r="C27">
+        <f>[1]Plan1!F14</f>
+        <v>40</v>
+      </c>
+      <c r="D27">
+        <v>0</v>
+      </c>
+      <c r="E27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>7</v>
+      </c>
+      <c r="B28">
+        <v>4</v>
+      </c>
+      <c r="C28">
+        <f>[1]Plan1!F15</f>
+        <v>40</v>
+      </c>
+      <c r="D28">
+        <v>0</v>
+      </c>
+      <c r="E28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>7</v>
+      </c>
+      <c r="B29">
+        <v>5</v>
+      </c>
+      <c r="C29">
+        <f>[1]Plan1!F16</f>
+        <v>40</v>
+      </c>
+      <c r="D29">
+        <v>0</v>
+      </c>
+      <c r="E29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>7</v>
+      </c>
+      <c r="B30">
+        <v>6</v>
+      </c>
+      <c r="C30">
+        <f>[1]Plan1!F17</f>
+        <v>40</v>
+      </c>
+      <c r="D30">
+        <v>0</v>
+      </c>
+      <c r="E30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>7</v>
+      </c>
+      <c r="B31">
+        <v>7</v>
+      </c>
+      <c r="C31">
+        <f>custos_talhao_103_parcela_196!F18</f>
+        <v>26690.924821300603</v>
+      </c>
+      <c r="D31">
+        <f>custos_talhao_103_parcela_196!F22</f>
+        <v>61593.637165760563</v>
+      </c>
+      <c r="E31">
+        <f>custos_talhao_103_parcela_196!F7</f>
+        <v>439.954551184004</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>8</v>
+      </c>
+      <c r="B32">
+        <v>0</v>
+      </c>
+      <c r="C32">
+        <f>[1]Plan1!G11</f>
+        <v>6000</v>
+      </c>
+      <c r="D32">
+        <v>0</v>
+      </c>
+      <c r="E32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>8</v>
+      </c>
+      <c r="B33">
+        <v>1</v>
+      </c>
+      <c r="C33">
+        <f>[1]Plan1!G12</f>
+        <v>290</v>
+      </c>
+      <c r="D33">
+        <v>0</v>
+      </c>
+      <c r="E33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>8</v>
+      </c>
+      <c r="B34">
+        <v>2</v>
+      </c>
+      <c r="C34">
+        <f>[1]Plan1!G13</f>
+        <v>140</v>
+      </c>
+      <c r="D34">
+        <v>0</v>
+      </c>
+      <c r="E34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>8</v>
+      </c>
+      <c r="B35">
+        <v>3</v>
+      </c>
+      <c r="C35">
+        <f>[1]Plan1!G14</f>
+        <v>40</v>
+      </c>
+      <c r="D35">
+        <v>0</v>
+      </c>
+      <c r="E35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>8</v>
+      </c>
+      <c r="B36">
+        <v>4</v>
+      </c>
+      <c r="C36">
+        <f>[1]Plan1!G15</f>
+        <v>40</v>
+      </c>
+      <c r="D36">
+        <v>0</v>
+      </c>
+      <c r="E36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>8</v>
+      </c>
+      <c r="B37">
+        <v>5</v>
+      </c>
+      <c r="C37">
+        <f>[1]Plan1!G16</f>
+        <v>40</v>
+      </c>
+      <c r="D37">
+        <v>0</v>
+      </c>
+      <c r="E37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>8</v>
+      </c>
+      <c r="B38">
+        <v>6</v>
+      </c>
+      <c r="C38">
+        <f>[1]Plan1!G17</f>
+        <v>40</v>
+      </c>
+      <c r="D38">
+        <v>0</v>
+      </c>
+      <c r="E38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>8</v>
+      </c>
+      <c r="B39">
+        <v>7</v>
+      </c>
+      <c r="C39">
+        <f>[1]Plan1!G18</f>
+        <v>40</v>
+      </c>
+      <c r="D39">
+        <v>0</v>
+      </c>
+      <c r="E39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>8</v>
+      </c>
+      <c r="B40">
+        <v>8</v>
+      </c>
+      <c r="C40">
+        <f>custos_talhao_103_parcela_196!G19</f>
+        <v>28800.731549927383</v>
+      </c>
+      <c r="D40">
+        <f>custos_talhao_103_parcela_196!G22</f>
+        <v>66772.827293603055</v>
+      </c>
+      <c r="E40">
+        <f>custos_talhao_103_parcela_196!G7</f>
+        <v>476.948766382879</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>9</v>
+      </c>
+      <c r="B41">
+        <v>0</v>
+      </c>
+      <c r="C41">
+        <f>[1]Plan1!H11</f>
+        <v>6000</v>
+      </c>
+      <c r="D41">
+        <v>0</v>
+      </c>
+      <c r="E41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>9</v>
+      </c>
+      <c r="B42">
+        <v>1</v>
+      </c>
+      <c r="C42">
+        <f>[1]Plan1!H12</f>
+        <v>290</v>
+      </c>
+      <c r="D42">
+        <v>0</v>
+      </c>
+      <c r="E42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>9</v>
+      </c>
+      <c r="B43">
+        <v>2</v>
+      </c>
+      <c r="C43">
+        <f>[1]Plan1!H13</f>
+        <v>140</v>
+      </c>
+      <c r="D43">
+        <v>0</v>
+      </c>
+      <c r="E43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>9</v>
+      </c>
+      <c r="B44">
+        <v>3</v>
+      </c>
+      <c r="C44">
+        <f>[1]Plan1!H14</f>
+        <v>40</v>
+      </c>
+      <c r="D44">
+        <v>0</v>
+      </c>
+      <c r="E44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>9</v>
+      </c>
+      <c r="B45">
+        <v>4</v>
+      </c>
+      <c r="C45">
+        <f>[1]Plan1!H15</f>
+        <v>40</v>
+      </c>
+      <c r="D45">
+        <v>0</v>
+      </c>
+      <c r="E45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>9</v>
+      </c>
+      <c r="B46">
+        <v>5</v>
+      </c>
+      <c r="C46">
+        <f>[1]Plan1!H16</f>
+        <v>40</v>
+      </c>
+      <c r="D46">
+        <v>0</v>
+      </c>
+      <c r="E46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>9</v>
+      </c>
+      <c r="B47">
+        <v>6</v>
+      </c>
+      <c r="C47">
+        <f>[1]Plan1!H17</f>
+        <v>40</v>
+      </c>
+      <c r="D47">
+        <v>0</v>
+      </c>
+      <c r="E47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>9</v>
+      </c>
+      <c r="B48">
+        <v>7</v>
+      </c>
+      <c r="C48">
+        <f>[1]Plan1!H18</f>
+        <v>40</v>
+      </c>
+      <c r="D48">
+        <v>0</v>
+      </c>
+      <c r="E48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>9</v>
+      </c>
+      <c r="B49">
+        <v>8</v>
+      </c>
+      <c r="C49">
+        <f>[1]Plan1!H19</f>
+        <v>40</v>
+      </c>
+      <c r="D49">
+        <v>0</v>
+      </c>
+      <c r="E49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>9</v>
+      </c>
+      <c r="B50">
+        <v>9</v>
+      </c>
+      <c r="C50">
+        <f>custos_talhao_103_parcela_196!H20</f>
+        <v>30563.598483896531</v>
+      </c>
+      <c r="D50">
+        <f>custos_talhao_103_parcela_196!H22</f>
+        <v>71100.343599826796</v>
+      </c>
+      <c r="E50">
+        <f>custos_talhao_103_parcela_196!H7</f>
+        <v>507.85959714161999</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>10</v>
+      </c>
+      <c r="B51">
+        <v>0</v>
+      </c>
+      <c r="C51">
+        <f>[1]Plan1!I11</f>
+        <v>6000</v>
+      </c>
+      <c r="D51">
+        <v>0</v>
+      </c>
+      <c r="E51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>10</v>
+      </c>
+      <c r="B52">
+        <v>1</v>
+      </c>
+      <c r="C52">
+        <f>[1]Plan1!I12</f>
+        <v>290</v>
+      </c>
+      <c r="D52">
+        <v>0</v>
+      </c>
+      <c r="E52">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>10</v>
+      </c>
+      <c r="B53">
+        <v>2</v>
+      </c>
+      <c r="C53">
+        <f>[1]Plan1!I13</f>
+        <v>140</v>
+      </c>
+      <c r="D53">
+        <v>0</v>
+      </c>
+      <c r="E53">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>10</v>
+      </c>
+      <c r="B54">
+        <v>3</v>
+      </c>
+      <c r="C54">
+        <f>[1]Plan1!I14</f>
+        <v>40</v>
+      </c>
+      <c r="D54">
+        <v>0</v>
+      </c>
+      <c r="E54">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>10</v>
+      </c>
+      <c r="B55">
+        <v>4</v>
+      </c>
+      <c r="C55">
+        <f>[1]Plan1!I15</f>
+        <v>40</v>
+      </c>
+      <c r="D55">
+        <v>0</v>
+      </c>
+      <c r="E55">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>10</v>
+      </c>
+      <c r="B56">
+        <v>5</v>
+      </c>
+      <c r="C56">
+        <f>[1]Plan1!I16</f>
+        <v>40</v>
+      </c>
+      <c r="D56">
+        <v>0</v>
+      </c>
+      <c r="E56">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>10</v>
+      </c>
+      <c r="B57">
+        <v>6</v>
+      </c>
+      <c r="C57">
+        <f>[1]Plan1!I17</f>
+        <v>40</v>
+      </c>
+      <c r="D57">
+        <v>0</v>
+      </c>
+      <c r="E57">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>10</v>
+      </c>
+      <c r="B58">
+        <v>7</v>
+      </c>
+      <c r="C58">
+        <f>[1]Plan1!I18</f>
+        <v>40</v>
+      </c>
+      <c r="D58">
+        <v>0</v>
+      </c>
+      <c r="E58">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>10</v>
+      </c>
+      <c r="B59">
+        <v>8</v>
+      </c>
+      <c r="C59">
+        <f>[1]Plan1!I19</f>
+        <v>40</v>
+      </c>
+      <c r="D59">
+        <v>0</v>
+      </c>
+      <c r="E59">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>10</v>
+      </c>
+      <c r="B60">
+        <v>9</v>
+      </c>
+      <c r="C60">
+        <f>[1]Plan1!I20</f>
+        <v>40</v>
+      </c>
+      <c r="D60">
+        <v>0</v>
+      </c>
+      <c r="E60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>10</v>
+      </c>
+      <c r="B61">
+        <v>10</v>
+      </c>
+      <c r="C61">
+        <f>custos_talhao_103_parcela_196!I21</f>
+        <v>32055.803763585376</v>
+      </c>
+      <c r="D61">
+        <f>custos_talhao_103_parcela_196!I22</f>
+        <v>74763.434985599917</v>
+      </c>
+      <c r="E61">
+        <f>custos_talhao_103_parcela_196!I7</f>
+        <v>534.02453561142795</v>
       </c>
     </row>
   </sheetData>

</xml_diff>